<commit_message>
fixed data set for ML
</commit_message>
<xml_diff>
--- a/basic.xlsx
+++ b/basic.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="50">
   <si>
     <t>Team</t>
   </si>
@@ -40,48 +40,57 @@
     <t>youngstown-state</t>
   </si>
   <si>
-    <t>2016-17</t>
+    <t>2017-18</t>
   </si>
   <si>
     <t>Cameron Morse</t>
   </si>
   <si>
+    <t>Braun Hartfield</t>
+  </si>
+  <si>
+    <t>Garrett Covington</t>
+  </si>
+  <si>
+    <t>Naz Bohannon</t>
+  </si>
+  <si>
+    <t>Tyree Robinson</t>
+  </si>
+  <si>
+    <t>Jaylen Benton</t>
+  </si>
+  <si>
+    <t>Devin Haygood</t>
+  </si>
+  <si>
+    <t>Jeremiah Ferguson</t>
+  </si>
+  <si>
+    <t>Michael Akuchie</t>
+  </si>
+  <si>
+    <t>Noe Anabir</t>
+  </si>
+  <si>
     <t>Francisco Santiago</t>
   </si>
   <si>
-    <t>Matt Donlan</t>
-  </si>
-  <si>
-    <t>Braun Hartfield</t>
-  </si>
-  <si>
-    <t>Jorden Kaufman</t>
-  </si>
-  <si>
-    <t>Devin Haygood</t>
-  </si>
-  <si>
-    <t>Brett Frantz</t>
-  </si>
-  <si>
-    <t>Latin Davis</t>
-  </si>
-  <si>
-    <t>Rahim Williams</t>
-  </si>
-  <si>
-    <t>Jeremiah Ferguson</t>
-  </si>
-  <si>
-    <t>Stefan Rosic</t>
-  </si>
-  <si>
-    <t>Tyler Warford</t>
-  </si>
-  <si>
     <t>Ryan Strollo</t>
   </si>
   <si>
+    <t>Jacob Brown</t>
+  </si>
+  <si>
+    <t>Dan Ritter</t>
+  </si>
+  <si>
+    <t>John Kirincic</t>
+  </si>
+  <si>
+    <t>Alex Wilbourn</t>
+  </si>
+  <si>
     <t>G</t>
   </si>
   <si>
@@ -94,52 +103,67 @@
     <t>74.0</t>
   </si>
   <si>
+    <t>76.0</t>
+  </si>
+  <si>
+    <t>77.0</t>
+  </si>
+  <si>
+    <t>78.0</t>
+  </si>
+  <si>
+    <t>75.0</t>
+  </si>
+  <si>
+    <t>79.0</t>
+  </si>
+  <si>
+    <t>80.0</t>
+  </si>
+  <si>
     <t>73.0</t>
   </si>
   <si>
-    <t>78.0</t>
-  </si>
-  <si>
-    <t>76.0</t>
+    <t>81.0</t>
   </si>
   <si>
     <t>84.0</t>
   </si>
   <si>
-    <t>79.0</t>
-  </si>
-  <si>
-    <t>75.0</t>
-  </si>
-  <si>
-    <t>71.0</t>
-  </si>
-  <si>
     <t>180</t>
   </si>
   <si>
+    <t>185</t>
+  </si>
+  <si>
+    <t>195</t>
+  </si>
+  <si>
+    <t>230</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>175</t>
+  </si>
+  <si>
+    <t>215</t>
+  </si>
+  <si>
+    <t>226</t>
+  </si>
+  <si>
     <t>160</t>
   </si>
   <si>
-    <t>185</t>
-  </si>
-  <si>
-    <t>250</t>
-  </si>
-  <si>
-    <t>175</t>
-  </si>
-  <si>
-    <t>165</t>
-  </si>
-  <si>
     <t>190</t>
   </si>
   <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>170</t>
+    <t>176</t>
+  </si>
+  <si>
+    <t>204</t>
   </si>
 </sst>
 </file>
@@ -497,7 +521,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -543,13 +567,13 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -569,13 +593,13 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -595,13 +619,13 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -621,13 +645,13 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H5" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -647,13 +671,13 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -673,13 +697,13 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -699,13 +723,13 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -725,10 +749,10 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H9" t="s">
         <v>38</v>
@@ -751,13 +775,13 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="H10" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -777,13 +801,13 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="H11" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -803,13 +827,13 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G12" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H12" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -829,13 +853,13 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H13" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -855,13 +879,91 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
         <v>22</v>
       </c>
-      <c r="G14" t="s">
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
         <v>25</v>
       </c>
-      <c r="H14" t="s">
-        <v>39</v>
+      <c r="G15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>